<commit_message>
Completed Database Setup and created tables.
</commit_message>
<xml_diff>
--- a/room_excel.xlsx
+++ b/room_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aztec\PycharmProjects\Hotel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32A24E1-4C02-44B5-9BB6-C1E41430096C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9CA746-13EF-42D5-860F-59F3CFF99452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{636D2328-66D0-4D71-AE89-2CB34CE7BB4E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Room Number</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Price</t>
-  </si>
-  <si>
-    <t>Availability</t>
   </si>
   <si>
     <t>A Class</t>
@@ -409,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5534E4B-E124-47FB-9CBC-867C47DF4179}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +420,7 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,148 +430,115 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>6000</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>6000</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>5000</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>5000</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>3000</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>201</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>6000</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>202</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>6000</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>203</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>4000</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>204</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>4000</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>205</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>3000</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>